<commit_message>
Added MOVE_RIGHTMOST as a start_pattern. Corrected AltsWithOnePattern to agree with description in Mancala Games by Russ. Corrected errors in Sadeqa and updated Sadeqa_II. Added games Sadeqa_III and Sadeqa_IV.
</commit_message>
<xml_diff>
--- a/test/fill_patterns.xlsx
+++ b/test/fill_patterns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF78A45D-A26E-4020-AB48-CC4269373BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DF30B1-254B-4E0C-8171-39D0EBF2443A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6525" yWindow="630" windowWidth="20520" windowHeight="15510" xr2:uid="{909EAA1E-1BAC-45CD-99EF-D1424EEE6150}"/>
+    <workbookView xWindow="2520" yWindow="510" windowWidth="25410" windowHeight="15510" xr2:uid="{909EAA1E-1BAC-45CD-99EF-D1424EEE6150}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,8 +429,8 @@
   <dimension ref="A1:Q93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E76" sqref="E76"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,7 +1215,7 @@
         <v>3</v>
       </c>
       <c r="C34" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" s="1">
         <f>SUM(E34:M35)</f>
@@ -1253,11 +1253,11 @@
         <v>4</v>
       </c>
       <c r="C36" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" s="1">
         <f>SUM(E36:M37)</f>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E36" s="1">
         <v>1</v>
@@ -1280,7 +1280,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G37" s="2">
         <v>0</v>
@@ -1297,7 +1297,7 @@
         <v>5</v>
       </c>
       <c r="C38" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="1">
         <f>SUM(E38:M39)</f>
@@ -1347,11 +1347,11 @@
         <v>6</v>
       </c>
       <c r="C40" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="1">
         <f>SUM(E40:M41)</f>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E40" s="1">
         <v>4</v>
@@ -1386,7 +1386,7 @@
         <v>0</v>
       </c>
       <c r="H41" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I41" s="2">
         <v>0</v>
@@ -1403,7 +1403,7 @@
         <v>3</v>
       </c>
       <c r="C42" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" s="1">
         <f>SUM(E42:M43)</f>
@@ -1441,11 +1441,11 @@
         <v>4</v>
       </c>
       <c r="C44" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" s="1">
         <f>SUM(E44:M45)</f>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E44" s="1">
         <v>4</v>
@@ -1454,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H44" s="1">
         <v>0</v>
@@ -1485,7 +1485,7 @@
         <v>5</v>
       </c>
       <c r="C46" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" s="1">
         <f>SUM(E46:M47)</f>
@@ -1535,11 +1535,11 @@
         <v>6</v>
       </c>
       <c r="C48" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" s="1">
         <f>SUM(E48:M49)</f>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E48" s="1">
         <v>4</v>
@@ -1548,7 +1548,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H48" s="1">
         <v>0</v>

</xml_diff>